<commit_message>
updating information to use only 16 binary vectors
</commit_message>
<xml_diff>
--- a/32/32_orthogonal_vectors.xlsx
+++ b/32/32_orthogonal_vectors.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\cogNeuroResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisweinberger/Documents/cogNeuroResearch/cogNeuro/32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62B5FD2-AE54-4CA5-BF76-94828B8B240B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7687CA74-FAF1-744D-86E3-B5AFF8FE832B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="32_orthogonal_vectors" sheetId="1" r:id="rId1"/>
-    <sheet name="PreviousVectors" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="PreviousVectors" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>Vector #</t>
   </si>
@@ -151,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,21 +1059,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH35" sqref="AH35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AH16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="30" width="3.28515625" customWidth="1"/>
-    <col min="31" max="33" width="2.85546875" customWidth="1"/>
-    <col min="37" max="37" width="3.7109375" customWidth="1"/>
-    <col min="38" max="38" width="3.85546875" customWidth="1"/>
-    <col min="39" max="69" width="3.7109375" customWidth="1"/>
+    <col min="3" max="30" width="3.33203125" customWidth="1"/>
+    <col min="31" max="33" width="2.83203125" customWidth="1"/>
+    <col min="37" max="37" width="3.6640625" customWidth="1"/>
+    <col min="38" max="38" width="3.83203125" customWidth="1"/>
+    <col min="39" max="69" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:69" ht="15.75" thickBot="1">
+    <row r="2" spans="1:69" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:69">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1576,7 +1577,7 @@
       <c r="BO4" s="5"/>
       <c r="BP4" s="5"/>
     </row>
-    <row r="5" spans="1:69">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1722,7 +1723,7 @@
       <c r="BO5" s="5"/>
       <c r="BP5" s="5"/>
     </row>
-    <row r="6" spans="1:69">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1870,7 +1871,7 @@
       <c r="BO6" s="5"/>
       <c r="BP6" s="5"/>
     </row>
-    <row r="7" spans="1:69">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2020,7 +2021,7 @@
       <c r="BO7" s="5"/>
       <c r="BP7" s="5"/>
     </row>
-    <row r="8" spans="1:69">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2172,7 +2173,7 @@
       <c r="BO8" s="5"/>
       <c r="BP8" s="5"/>
     </row>
-    <row r="9" spans="1:69">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2326,7 +2327,7 @@
       <c r="BO9" s="5"/>
       <c r="BP9" s="5"/>
     </row>
-    <row r="10" spans="1:69">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2482,7 +2483,7 @@
       <c r="BO10" s="5"/>
       <c r="BP10" s="5"/>
     </row>
-    <row r="11" spans="1:69">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2640,7 +2641,7 @@
       <c r="BO11" s="5"/>
       <c r="BP11" s="5"/>
     </row>
-    <row r="12" spans="1:69">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2800,7 +2801,7 @@
       <c r="BO12" s="5"/>
       <c r="BP12" s="5"/>
     </row>
-    <row r="13" spans="1:69">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2962,7 +2963,7 @@
       <c r="BO13" s="5"/>
       <c r="BP13" s="5"/>
     </row>
-    <row r="14" spans="1:69">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3126,7 +3127,7 @@
       <c r="BO14" s="5"/>
       <c r="BP14" s="5"/>
     </row>
-    <row r="15" spans="1:69">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3292,7 +3293,7 @@
       <c r="BO15" s="5"/>
       <c r="BP15" s="5"/>
     </row>
-    <row r="16" spans="1:69">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3460,7 +3461,7 @@
       <c r="BO16" s="5"/>
       <c r="BP16" s="5"/>
     </row>
-    <row r="17" spans="1:68">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3630,7 +3631,7 @@
       <c r="BO17" s="5"/>
       <c r="BP17" s="5"/>
     </row>
-    <row r="18" spans="1:68">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3802,7 +3803,7 @@
       <c r="BO18" s="5"/>
       <c r="BP18" s="5"/>
     </row>
-    <row r="19" spans="1:68">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3976,7 +3977,7 @@
       <c r="BO19" s="5"/>
       <c r="BP19" s="5"/>
     </row>
-    <row r="20" spans="1:68">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4152,7 +4153,7 @@
       <c r="BO20" s="5"/>
       <c r="BP20" s="5"/>
     </row>
-    <row r="21" spans="1:68">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4330,7 +4331,7 @@
       <c r="BO21" s="5"/>
       <c r="BP21" s="5"/>
     </row>
-    <row r="22" spans="1:68">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4510,7 +4511,7 @@
       <c r="BO22" s="5"/>
       <c r="BP22" s="5"/>
     </row>
-    <row r="23" spans="1:68">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4692,7 +4693,7 @@
       <c r="BO23" s="5"/>
       <c r="BP23" s="5"/>
     </row>
-    <row r="24" spans="1:68">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4876,7 +4877,7 @@
       <c r="BO24" s="5"/>
       <c r="BP24" s="5"/>
     </row>
-    <row r="25" spans="1:68">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5062,7 +5063,7 @@
       <c r="BO25" s="5"/>
       <c r="BP25" s="5"/>
     </row>
-    <row r="26" spans="1:68">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5250,7 +5251,7 @@
       <c r="BO26" s="5"/>
       <c r="BP26" s="5"/>
     </row>
-    <row r="27" spans="1:68">
+    <row r="27" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5440,7 +5441,7 @@
       <c r="BO27" s="5"/>
       <c r="BP27" s="5"/>
     </row>
-    <row r="28" spans="1:68">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5632,7 +5633,7 @@
       <c r="BO28" s="5"/>
       <c r="BP28" s="5"/>
     </row>
-    <row r="29" spans="1:68">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5826,7 +5827,7 @@
       <c r="BO29" s="5"/>
       <c r="BP29" s="5"/>
     </row>
-    <row r="30" spans="1:68">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6022,7 +6023,7 @@
       <c r="BO30" s="5"/>
       <c r="BP30" s="5"/>
     </row>
-    <row r="31" spans="1:68">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6220,7 +6221,7 @@
       <c r="BO31" s="5"/>
       <c r="BP31" s="5"/>
     </row>
-    <row r="32" spans="1:68">
+    <row r="32" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6420,7 +6421,7 @@
       <c r="BO32" s="5"/>
       <c r="BP32" s="5"/>
     </row>
-    <row r="33" spans="1:68">
+    <row r="33" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6622,7 +6623,7 @@
       </c>
       <c r="BP33" s="5"/>
     </row>
-    <row r="34" spans="1:68" ht="15.75" thickBot="1">
+    <row r="34" spans="1:68" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AJ34">
         <v>32</v>
       </c>
@@ -6724,7 +6725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:68" ht="15.75" thickBot="1">
+    <row r="35" spans="1:68" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AK35" s="6" t="s">
         <v>37</v>
       </c>
@@ -6735,6 +6736,1611 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FB9BBF-A830-4A49-A928-6FC800AAC279}">
+  <dimension ref="A1:AH16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="33" width="3.33203125" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <f>SUM(B2:AG2)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" ref="AH3:AH16" si="0">SUM(B3:AG3)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>1</v>
+      </c>
+      <c r="AE12">
+        <v>1</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BQ34"/>
   <sheetViews>
@@ -6742,13 +8348,13 @@
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="33" width="3.5703125" customWidth="1"/>
-    <col min="38" max="69" width="3.28515625" customWidth="1"/>
+    <col min="2" max="33" width="3.5" customWidth="1"/>
+    <col min="38" max="69" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="31.5" thickBot="1">
+    <row r="1" spans="1:69" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6793,7 +8399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:69" ht="16.5" thickBot="1">
+    <row r="2" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -6994,7 +8600,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:69" ht="16.5" thickBot="1">
+    <row r="3" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -7135,7 +8741,7 @@
       <c r="BP3" s="5"/>
       <c r="BQ3" s="5"/>
     </row>
-    <row r="4" spans="1:69" ht="16.5" thickBot="1">
+    <row r="4" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -7279,7 +8885,7 @@
       <c r="BP4" s="5"/>
       <c r="BQ4" s="5"/>
     </row>
-    <row r="5" spans="1:69" ht="16.5" thickBot="1">
+    <row r="5" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -7425,7 +9031,7 @@
       <c r="BP5" s="5"/>
       <c r="BQ5" s="5"/>
     </row>
-    <row r="6" spans="1:69" ht="16.5" thickBot="1">
+    <row r="6" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -7573,7 +9179,7 @@
       <c r="BP6" s="5"/>
       <c r="BQ6" s="5"/>
     </row>
-    <row r="7" spans="1:69" ht="16.5" thickBot="1">
+    <row r="7" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -7723,7 +9329,7 @@
       <c r="BP7" s="5"/>
       <c r="BQ7" s="5"/>
     </row>
-    <row r="8" spans="1:69" ht="16.5" thickBot="1">
+    <row r="8" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -7874,7 +9480,7 @@
       <c r="BP8" s="5"/>
       <c r="BQ8" s="5"/>
     </row>
-    <row r="9" spans="1:69" ht="16.5" thickBot="1">
+    <row r="9" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8027,7 +9633,7 @@
       <c r="BP9" s="5"/>
       <c r="BQ9" s="5"/>
     </row>
-    <row r="10" spans="1:69" ht="16.5" thickBot="1">
+    <row r="10" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8182,7 +9788,7 @@
       <c r="BP10" s="5"/>
       <c r="BQ10" s="5"/>
     </row>
-    <row r="11" spans="1:69" ht="16.5" thickBot="1">
+    <row r="11" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8339,7 +9945,7 @@
       <c r="BP11" s="5"/>
       <c r="BQ11" s="5"/>
     </row>
-    <row r="12" spans="1:69" ht="16.5" thickBot="1">
+    <row r="12" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8498,7 +10104,7 @@
       <c r="BP12" s="5"/>
       <c r="BQ12" s="5"/>
     </row>
-    <row r="13" spans="1:69" ht="16.5" thickBot="1">
+    <row r="13" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8659,7 +10265,7 @@
       <c r="BP13" s="5"/>
       <c r="BQ13" s="5"/>
     </row>
-    <row r="14" spans="1:69" ht="16.5" thickBot="1">
+    <row r="14" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8822,7 +10428,7 @@
       <c r="BP14" s="5"/>
       <c r="BQ14" s="5"/>
     </row>
-    <row r="15" spans="1:69" ht="16.5" thickBot="1">
+    <row r="15" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8987,7 +10593,7 @@
       <c r="BP15" s="5"/>
       <c r="BQ15" s="5"/>
     </row>
-    <row r="16" spans="1:69" ht="16.5" thickBot="1">
+    <row r="16" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9154,7 +10760,7 @@
       <c r="BP16" s="5"/>
       <c r="BQ16" s="5"/>
     </row>
-    <row r="17" spans="1:69" ht="16.5" thickBot="1">
+    <row r="17" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -9323,7 +10929,7 @@
       <c r="BP17" s="5"/>
       <c r="BQ17" s="5"/>
     </row>
-    <row r="18" spans="1:69" ht="16.5" thickBot="1">
+    <row r="18" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -9494,7 +11100,7 @@
       <c r="BP18" s="5"/>
       <c r="BQ18" s="5"/>
     </row>
-    <row r="19" spans="1:69" ht="16.5" thickBot="1">
+    <row r="19" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -9667,7 +11273,7 @@
       <c r="BP19" s="5"/>
       <c r="BQ19" s="5"/>
     </row>
-    <row r="20" spans="1:69" ht="16.5" thickBot="1">
+    <row r="20" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -9842,7 +11448,7 @@
       <c r="BP20" s="5"/>
       <c r="BQ20" s="5"/>
     </row>
-    <row r="21" spans="1:69" ht="16.5" thickBot="1">
+    <row r="21" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -10019,7 +11625,7 @@
       <c r="BP21" s="5"/>
       <c r="BQ21" s="5"/>
     </row>
-    <row r="22" spans="1:69" ht="16.5" thickBot="1">
+    <row r="22" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -10198,7 +11804,7 @@
       <c r="BP22" s="5"/>
       <c r="BQ22" s="5"/>
     </row>
-    <row r="23" spans="1:69" ht="16.5" thickBot="1">
+    <row r="23" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -10379,7 +11985,7 @@
       <c r="BP23" s="5"/>
       <c r="BQ23" s="5"/>
     </row>
-    <row r="24" spans="1:69" ht="16.5" thickBot="1">
+    <row r="24" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -10562,7 +12168,7 @@
       <c r="BP24" s="5"/>
       <c r="BQ24" s="5"/>
     </row>
-    <row r="25" spans="1:69" ht="16.5" thickBot="1">
+    <row r="25" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -10747,7 +12353,7 @@
       <c r="BP25" s="5"/>
       <c r="BQ25" s="5"/>
     </row>
-    <row r="26" spans="1:69" ht="16.5" thickBot="1">
+    <row r="26" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -10934,7 +12540,7 @@
       <c r="BP26" s="5"/>
       <c r="BQ26" s="5"/>
     </row>
-    <row r="27" spans="1:69" ht="16.5" thickBot="1">
+    <row r="27" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -11123,7 +12729,7 @@
       <c r="BP27" s="5"/>
       <c r="BQ27" s="5"/>
     </row>
-    <row r="28" spans="1:69" ht="16.5" thickBot="1">
+    <row r="28" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -11314,7 +12920,7 @@
       <c r="BP28" s="5"/>
       <c r="BQ28" s="5"/>
     </row>
-    <row r="29" spans="1:69" ht="16.5" thickBot="1">
+    <row r="29" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -11507,7 +13113,7 @@
       <c r="BP29" s="5"/>
       <c r="BQ29" s="5"/>
     </row>
-    <row r="30" spans="1:69" ht="16.5" thickBot="1">
+    <row r="30" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -11702,7 +13308,7 @@
       <c r="BP30" s="5"/>
       <c r="BQ30" s="5"/>
     </row>
-    <row r="31" spans="1:69" ht="16.5" thickBot="1">
+    <row r="31" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -11899,7 +13505,7 @@
       <c r="BP31" s="5"/>
       <c r="BQ31" s="5"/>
     </row>
-    <row r="32" spans="1:69" ht="16.5" thickBot="1">
+    <row r="32" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -12098,7 +13704,7 @@
       <c r="BP32" s="5"/>
       <c r="BQ32" s="5"/>
     </row>
-    <row r="33" spans="1:69" ht="16.5" thickBot="1">
+    <row r="33" spans="1:69" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -12299,7 +13905,7 @@
       </c>
       <c r="BQ33" s="5"/>
     </row>
-    <row r="34" spans="1:69" ht="15.75" thickBot="1">
+    <row r="34" spans="1:69" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AK34" s="6" t="s">
         <v>34</v>
       </c>

</xml_diff>